<commit_message>
set up focus on working sheet when excel file opens, added some comments
</commit_message>
<xml_diff>
--- a/chemolisty.xlsx
+++ b/chemolisty.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\naucse-python\onkologie\"/>
@@ -1395,6 +1395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -1567,7 +1568,7 @@
       </c>
       <c r="D12" s="18">
         <f ca="1">TODAY()+1</f>
-        <v>44727</v>
+        <v>44736</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
@@ -1681,7 +1682,7 @@
       </c>
       <c r="C19" s="28">
         <f ca="1">D12+F10</f>
-        <v>44741</v>
+        <v>44750</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1834,6 +1835,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -2009,7 +2011,7 @@
       </c>
       <c r="D12" s="18">
         <f ca="1">TODAY()+1</f>
-        <v>44727</v>
+        <v>44736</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
@@ -2104,7 +2106,7 @@
       </c>
       <c r="C18" s="76">
         <f ca="1">D12+G10</f>
-        <v>44741</v>
+        <v>44750</v>
       </c>
       <c r="D18" s="47"/>
       <c r="E18" s="47"/>
@@ -2273,6 +2275,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
@@ -2438,7 +2441,7 @@
       </c>
       <c r="D11" s="65">
         <f ca="1">TODAY()+1</f>
-        <v>44727</v>
+        <v>44736</v>
       </c>
       <c r="E11" s="66"/>
       <c r="F11" s="67"/>
@@ -2550,7 +2553,7 @@
       </c>
       <c r="C18" s="76">
         <f ca="1">D11+F8</f>
-        <v>44727</v>
+        <v>44736</v>
       </c>
       <c r="D18" s="47"/>
       <c r="E18" s="47"/>
@@ -2741,6 +2744,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -2995,7 +2999,7 @@
       </c>
       <c r="D16" s="134">
         <f ca="1">TODAY()+1</f>
-        <v>44727</v>
+        <v>44736</v>
       </c>
       <c r="E16" s="66"/>
       <c r="F16" s="67"/>
@@ -3056,7 +3060,7 @@
       </c>
       <c r="C20" s="76">
         <f ca="1">D16+F14</f>
-        <v>44748</v>
+        <v>44757</v>
       </c>
       <c r="D20" s="46"/>
       <c r="E20" s="46"/>
@@ -3235,6 +3239,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -3416,7 +3421,7 @@
       </c>
       <c r="D13" s="65">
         <f ca="1">TODAY()+1</f>
-        <v>44727</v>
+        <v>44736</v>
       </c>
       <c r="E13" s="73"/>
       <c r="F13" s="73"/>
@@ -3480,7 +3485,7 @@
       </c>
       <c r="C18" s="76">
         <f ca="1">D13+F10</f>
-        <v>44748</v>
+        <v>44757</v>
       </c>
       <c r="D18" s="46"/>
       <c r="E18" s="46"/>

</xml_diff>